<commit_message>
newest verstion and some results
</commit_message>
<xml_diff>
--- a/server_version/time_change.xlsx
+++ b/server_version/time_change.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam Wagner\Documents\Masterarbeit\PythonCode\server_version\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B854E792-A6F2-40A3-8F5A-E9B547B6B122}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB87A2F1-0E4D-4F99-A2C9-91AC5C069CF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{75652EE4-C3E7-4CC1-90CF-F4E25FA2E9D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
+    <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="335">
   <si>
     <t>Seq_count variant for l = 1 is running,,,</t>
   </si>
@@ -763,370 +764,280 @@
     <t>time win</t>
   </si>
   <si>
-    <t>Set variant for l = 1 is running...</t>
-  </si>
-  <si>
-    <t>set_1_20_0.1_0.5:1.6857974529266357</t>
-  </si>
-  <si>
-    <t>set_1_20_0.4_0.5:1.6809136867523193</t>
-  </si>
-  <si>
-    <t>set_1_20_0.6_0.5:1.778003215789795</t>
-  </si>
-  <si>
-    <t>set_1_160_0.1_0.5:1.8245296478271484</t>
-  </si>
-  <si>
-    <t>set_1_160_0.4_0.5:1.9450786113739014</t>
-  </si>
-  <si>
-    <t>set_1_160_0.6_0.5:1.8875980377197266</t>
-  </si>
-  <si>
-    <t>set_1_20_0.1_0.9:1.5600755214691162</t>
-  </si>
-  <si>
-    <t>set_1_20_0.4_0.9:1.817366600036621</t>
-  </si>
-  <si>
-    <t>set_1_20_0.6_0.9:2.0141279697418213</t>
-  </si>
-  <si>
-    <t>set_1_160_0.1_0.9:1.6152708530426025</t>
-  </si>
-  <si>
-    <t>set_1_160_0.4_0.9:1.5918633937835693</t>
-  </si>
-  <si>
-    <t>set_1_160_0.6_0.9:1.8430287837982178</t>
-  </si>
-  <si>
-    <t>Set variant for l = 3 is running...</t>
-  </si>
-  <si>
-    <t>set_3_20_0.1_0.5:1.4508326053619385</t>
-  </si>
-  <si>
-    <t>set_3_20_0.4_0.5:4.652474880218506</t>
-  </si>
-  <si>
-    <t>set_3_20_0.6_0.5:4.835260391235352</t>
-  </si>
-  <si>
-    <t>set_3_160_0.1_0.5:1.6296799182891846</t>
-  </si>
-  <si>
-    <t>set_3_160_0.4_0.5:3.365975856781006</t>
-  </si>
-  <si>
-    <t>set_3_160_0.6_0.5:3.272418975830078</t>
-  </si>
-  <si>
-    <t>set_3_20_0.1_0.9:1.4714770317077637</t>
-  </si>
-  <si>
-    <t>set_3_20_0.4_0.9:5.05855131149292</t>
-  </si>
-  <si>
-    <t>set_3_20_0.6_0.9:6.322547674179077</t>
-  </si>
-  <si>
-    <t>set_3_160_0.1_0.9:2.242349147796631</t>
-  </si>
-  <si>
-    <t>set_3_160_0.4_0.9:4.764561653137207</t>
-  </si>
-  <si>
-    <t>set_3_160_0.6_0.9:4.459415674209595</t>
-  </si>
-  <si>
-    <t>C:\Users\Miriam Wagner\AppData\Local\Programs\Python\Python36\python.exe "C:/Users/Miriam Wagner/Documents/Masterarbeit/PythonCode/server_version/runtime_test.py"</t>
-  </si>
-  <si>
-    <t>Set_count variant for l = 1 is running...</t>
-  </si>
-  <si>
-    <t>set_count_1_20_0.1_0.5:3.8300678730010986</t>
-  </si>
-  <si>
-    <t>set_count_1_20_0.4_0.5:4.012199878692627</t>
-  </si>
-  <si>
-    <t>set_count_1_20_0.6_0.5:3.8441522121429443</t>
-  </si>
-  <si>
-    <t>set_count_1_160_0.1_0.5:4.312342405319214</t>
-  </si>
-  <si>
-    <t>set_count_1_160_0.4_0.5:4.065478324890137</t>
-  </si>
-  <si>
-    <t>set_count_1_160_0.6_0.5:4.231999635696411</t>
-  </si>
-  <si>
-    <t>set_count_1_20_0.1_0.9:3.4664154052734375</t>
-  </si>
-  <si>
-    <t>set_count_1_20_0.4_0.9:2.21433162689209</t>
-  </si>
-  <si>
-    <t>set_count_1_20_0.6_0.9:2.6532278060913086</t>
-  </si>
-  <si>
-    <t>set_count_1_160_0.1_0.9:2.2639787197113037</t>
-  </si>
-  <si>
-    <t>set_count_1_160_0.4_0.9:2.4980709552764893</t>
-  </si>
-  <si>
-    <t>set_count_1_160_0.6_0.9:2.2948737144470215</t>
-  </si>
-  <si>
-    <t>Set_count variant for l = 3 is running...</t>
-  </si>
-  <si>
-    <t>set_count_3_20_0.1_0.5:2.9051787853240967</t>
-  </si>
-  <si>
-    <t>set_count_3_20_0.4_0.5:346.88626980781555</t>
-  </si>
-  <si>
-    <t>set_count_3_20_0.6_0.5:609.6414766311646</t>
-  </si>
-  <si>
-    <t>set_count_3_160_0.1_0.5:4.051259994506836</t>
-  </si>
-  <si>
-    <t>set_count_3_160_0.4_0.5:12.465900897979736</t>
-  </si>
-  <si>
-    <t>set_count_3_160_0.6_0.5:12.525901794433594</t>
-  </si>
-  <si>
-    <t>set_count_3_20_0.1_0.9:3.635695695877075</t>
-  </si>
-  <si>
-    <t>set_count_3_20_0.4_0.9:369.38288593292236</t>
-  </si>
-  <si>
-    <t>set_count_3_20_0.6_0.9:326.8877441883087</t>
-  </si>
-  <si>
-    <t>set_count_3_160_0.1_0.9:1.7495553493499756</t>
-  </si>
-  <si>
-    <t>set_count_3_160_0.4_0.9:6.092363595962524</t>
-  </si>
-  <si>
-    <t>set_count_3_160_0.6_0.9:5.8266966342926025</t>
-  </si>
-  <si>
-    <t>Seq_count variant for l = 1 is running...</t>
-  </si>
-  <si>
-    <t>violating</t>
-  </si>
-  <si>
-    <t>0.2031083106994629</t>
-  </si>
-  <si>
-    <t>seq_count_1_20_0.1_0.5:4.030297040939331</t>
-  </si>
-  <si>
-    <t>0.21873021125793457</t>
-  </si>
-  <si>
-    <t>seq_count_1_20_0.4_0.5:3.9522206783294678</t>
-  </si>
-  <si>
-    <t>0.2030773162841797</t>
-  </si>
-  <si>
-    <t>seq_count_1_20_0.6_0.5:3.9521634578704834</t>
-  </si>
-  <si>
-    <t>0.2031080722808838</t>
-  </si>
-  <si>
-    <t>seq_count_1_160_0.1_0.5:4.217750549316406</t>
-  </si>
-  <si>
-    <t>0.23435187339782715</t>
-  </si>
-  <si>
-    <t>seq_count_1_160_0.4_0.5:4.061577558517456</t>
-  </si>
-  <si>
-    <t>0.21869826316833496</t>
-  </si>
-  <si>
-    <t>seq_count_1_160_0.6_0.5:4.108404874801636</t>
-  </si>
-  <si>
-    <t>seq_count_1_20_0.1_0.9:1.749589204788208</t>
-  </si>
-  <si>
-    <t>0.18745636940002441</t>
-  </si>
-  <si>
-    <t>seq_count_1_20_0.4_0.9:1.640230417251587</t>
-  </si>
-  <si>
-    <t>0.21866941452026367</t>
-  </si>
-  <si>
-    <t>seq_count_1_20_0.6_0.9:1.6544482707977295</t>
-  </si>
-  <si>
-    <t>0.23429059982299805</t>
-  </si>
-  <si>
-    <t>seq_count_1_160_0.1_0.9:1.7808289527893066</t>
-  </si>
-  <si>
-    <t>0.40615272521972656</t>
-  </si>
-  <si>
-    <t>seq_count_1_160_0.4_0.9:2.062013626098633</t>
-  </si>
-  <si>
-    <t>0.21870803833007812</t>
-  </si>
-  <si>
-    <t>seq_count_1_160_0.6_0.9:1.7626423835754395</t>
-  </si>
-  <si>
-    <t>Seq_count variant for l = 3 is running...</t>
-  </si>
-  <si>
-    <t>0.20307016372680664</t>
-  </si>
-  <si>
-    <t>seq_count_3_20_0.1_0.5:4.200779676437378</t>
-  </si>
-  <si>
-    <t>seq_count_3_20_0.4_0.5:14.189681053161621</t>
-  </si>
-  <si>
-    <t>seq_count_3_20_0.6_0.5:17.321147680282593</t>
-  </si>
-  <si>
-    <t>0.21869707107543945</t>
-  </si>
-  <si>
-    <t>seq_count_3_160_0.1_0.5:4.184560537338257</t>
-  </si>
-  <si>
-    <t>seq_count_3_160_0.4_0.5:5.85058069229126</t>
-  </si>
-  <si>
-    <t>seq_count_3_160_0.6_0.5:5.919343709945679</t>
-  </si>
-  <si>
-    <t>0.20304298400878906</t>
-  </si>
-  <si>
-    <t>seq_count_3_20_0.1_0.9:1.7578601837158203</t>
-  </si>
-  <si>
-    <t>seq_count_3_20_0.4_0.9:11.605495929718018</t>
-  </si>
-  <si>
-    <t>seq_count_3_20_0.6_0.9:14.93086552619934</t>
-  </si>
-  <si>
-    <t>0.20311331748962402</t>
-  </si>
-  <si>
-    <t>seq_count_3_160_0.1_0.9:1.7783782482147217</t>
-  </si>
-  <si>
-    <t>seq_count_3_160_0.4_0.9:3.5441079139709473</t>
-  </si>
-  <si>
-    <t>seq_count_3_160_0.6_0.9:3.507115602493286</t>
-  </si>
-  <si>
-    <t>Seq_time variant for l = 1 is running...</t>
-  </si>
-  <si>
-    <t>seq_time_1_20_0.1_0.5:12.554085731506348</t>
-  </si>
-  <si>
-    <t>seq_time_1_20_0.4_0.5:12.745370626449585</t>
-  </si>
-  <si>
-    <t>seq_time_1_20_0.6_0.5:12.760683059692383</t>
-  </si>
-  <si>
-    <t>seq_time_1_160_0.1_0.5:12.620474576950073</t>
-  </si>
-  <si>
-    <t>seq_time_1_160_0.4_0.5:13.760821104049683</t>
-  </si>
-  <si>
-    <t>seq_time_1_160_0.6_0.5:13.807446241378784</t>
-  </si>
-  <si>
-    <t>seq_time_1_20_0.1_0.9:12.5892915725708</t>
-  </si>
-  <si>
-    <t>seq_time_1_20_0.4_0.9:13.042328119277954</t>
-  </si>
-  <si>
-    <t>seq_time_1_20_0.6_0.9:12.714251279830933</t>
-  </si>
-  <si>
-    <t>seq_time_1_160_0.1_0.9:12.48079228401184</t>
-  </si>
-  <si>
-    <t>seq_time_1_160_0.4_0.9:13.496390342712402</t>
-  </si>
-  <si>
-    <t>seq_time_1_160_0.6_0.9:13.075347185134888</t>
-  </si>
-  <si>
-    <t>Seq_time variant for l = 3 is running...</t>
-  </si>
-  <si>
-    <t>seq_time_3_20_0.1_0.5:13.77666425704956</t>
-  </si>
-  <si>
-    <t>seq_time_3_20_0.4_0.5:17.16761350631714</t>
-  </si>
-  <si>
-    <t>seq_time_3_20_0.6_0.5:17.759673357009888</t>
-  </si>
-  <si>
-    <t>seq_time_3_160_0.1_0.5:13.199344158172607</t>
-  </si>
-  <si>
-    <t>seq_time_3_160_0.4_0.5:11.558161973953247</t>
-  </si>
-  <si>
-    <t>seq_time_3_160_0.6_0.5:11.495925188064575</t>
-  </si>
-  <si>
-    <t>seq_time_3_20_0.1_0.9:13.382518529891968</t>
-  </si>
-  <si>
-    <t>seq_time_3_20_0.4_0.9:17.400565147399902</t>
-  </si>
-  <si>
-    <t>seq_time_3_20_0.6_0.9:17.698682069778442</t>
-  </si>
-  <si>
-    <t>seq_time_3_160_0.1_0.9:13.02665090560913</t>
-  </si>
-  <si>
-    <t>seq_time_3_160_0.4_0.9:11.654093027114868</t>
-  </si>
-  <si>
-    <t>seq_time_3_160_0.6_0.9:11.412866353988647</t>
-  </si>
-  <si>
     <t>Process finished with exit code 0</t>
+  </si>
+  <si>
+    <t>Set variant for l = 1 is running,,,</t>
+  </si>
+  <si>
+    <t>Set variant for l = 3 is running,,,</t>
+  </si>
+  <si>
+    <t>Set_count variant for l = 1 is running,,,</t>
+  </si>
+  <si>
+    <t>Set_count variant for l = 3 is running,,,</t>
+  </si>
+  <si>
+    <t>Seq_count variant for l = 3 is running,,,</t>
+  </si>
+  <si>
+    <t>Seq_time variant for l = 1 is running,,,</t>
+  </si>
+  <si>
+    <t>Seq_time variant for l = 3 is running,,,</t>
+  </si>
+  <si>
+    <t>set_1_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_1_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_1_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_1_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_1_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_1_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_1_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_1_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_1_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_1_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_1_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_1_160_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_3_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_3_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_3_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_3_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_3_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_3_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_3_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_3_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_3_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_3_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_3_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_3_160_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_count_1_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_count_1_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_count_1_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_count_1_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_count_1_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_count_1_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_count_1_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_count_1_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_count_1_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_count_1_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_count_1_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_count_1_160_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_count_3_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_count_3_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_count_3_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_count_3_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>set_count_3_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>set_count_3_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>set_count_3_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_count_3_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_count_3_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>set_count_3_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>set_count_3_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>set_count_3_160_0,6_0,9</t>
+  </si>
+  <si>
+    <t>seq_count_3_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>seq_count_3_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>seq_count_3_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>seq_count_3_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>seq_count_3_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>seq_count_3_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>seq_count_3_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>seq_count_3_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>seq_count_3_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>seq_count_3_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>seq_count_3_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>seq_count_3_160_0,6_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_1_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_1_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_1_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_1_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_1_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_1_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_1_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_1_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_1_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_1_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_1_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_1_160_0,6_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_3_20_0,1_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_3_20_0,4_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_3_20_0,6_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_3_160_0,1_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_3_160_0,4_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_3_160_0,6_0,5</t>
+  </si>
+  <si>
+    <t>seq_time_3_20_0,1_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_3_20_0,4_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_3_20_0,6_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_3_160_0,1_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_3_160_0,4_0,9</t>
+  </si>
+  <si>
+    <t>seq_time_3_160_0,6_0,9</t>
   </si>
 </sst>
 </file>
@@ -1170,13 +1081,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1493,8 +1403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772FAE4-513F-4E3C-9DB1-6F49BBF1CB03}">
   <dimension ref="A1:E483"/>
   <sheetViews>
-    <sheetView topLeftCell="A449" workbookViewId="0">
-      <selection activeCell="B483" sqref="B483"/>
+    <sheetView topLeftCell="A237" workbookViewId="0">
+      <selection activeCell="C242" sqref="C242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10184,785 +10094,992 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73DD8F1F-F77E-4E23-8C2D-3B08AC8324BD}">
-  <dimension ref="A1:A155"/>
+  <dimension ref="A1:E106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:A155"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="D1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="B2">
+        <v>1.68579745292663</v>
+      </c>
+      <c r="D2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2">
+        <v>2.5306429862975999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3">
+        <v>1.68091368675231</v>
+      </c>
+      <c r="D3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E3">
+        <v>2.7337298393249498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B4">
+        <v>1.77800321578979</v>
+      </c>
+      <c r="D4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E4">
+        <v>2.6712467670440598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>254</v>
+      </c>
+      <c r="B5">
+        <v>1.82452964782714</v>
+      </c>
+      <c r="D5" t="s">
+        <v>254</v>
+      </c>
+      <c r="E5">
+        <v>2.63999938964843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6">
+        <v>1.9450786113739</v>
+      </c>
+      <c r="D6" t="s">
+        <v>255</v>
+      </c>
+      <c r="E6">
+        <v>2.7024869918823198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B7">
+        <v>1.8875980377197199</v>
+      </c>
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E7">
+        <v>3.7803606986999498</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8">
+        <v>1.56007552146911</v>
+      </c>
+      <c r="D8" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8">
+        <v>3.2804718017578098</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9">
+        <v>1.81736660003662</v>
+      </c>
+      <c r="D9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9">
+        <v>3.4054498672485298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>259</v>
+      </c>
+      <c r="B10">
+        <v>2.01412796974182</v>
+      </c>
+      <c r="D10" t="s">
+        <v>259</v>
+      </c>
+      <c r="E10">
+        <v>3.6710045337677002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B11">
+        <v>1.6152708530426001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>260</v>
+      </c>
+      <c r="E11">
+        <v>4.0927813053131104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>261</v>
+      </c>
+      <c r="B12">
+        <v>1.59186339378356</v>
+      </c>
+      <c r="D12" t="s">
+        <v>261</v>
+      </c>
+      <c r="E12">
+        <v>3.6085228919982901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>262</v>
+      </c>
+      <c r="B13">
+        <v>1.84302878379821</v>
+      </c>
+      <c r="D13" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13">
+        <v>3.4210674762725799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="D14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15">
+        <v>1.45083260536193</v>
+      </c>
+      <c r="D15" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15">
+        <v>3.3585848808288499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>264</v>
+      </c>
+      <c r="B16">
+        <v>4.6524748802184996</v>
+      </c>
+      <c r="D16" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16">
+        <v>6.3734900951385498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17">
+        <v>4.8352603912353498</v>
+      </c>
+      <c r="D17" t="s">
+        <v>265</v>
+      </c>
+      <c r="E17">
+        <v>9.15409207344055</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>266</v>
+      </c>
+      <c r="B18">
+        <v>1.6296799182891799</v>
+      </c>
+      <c r="D18" t="s">
+        <v>266</v>
+      </c>
+      <c r="E18">
+        <v>3.67100477218627</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B19">
+        <v>3.3659758567810001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>267</v>
+      </c>
+      <c r="E19">
+        <v>4.9050917625427202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B20">
+        <v>3.2724189758300701</v>
+      </c>
+      <c r="D20" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20">
+        <v>4.9207141399383501</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B21">
+        <v>1.4714770317077599</v>
+      </c>
+      <c r="D21" t="s">
+        <v>269</v>
+      </c>
+      <c r="E21">
+        <v>3.9678108692169101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>270</v>
+      </c>
+      <c r="B22">
+        <v>5.0585513114929199</v>
+      </c>
+      <c r="D22" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22">
+        <v>7.5607149600982604</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>271</v>
+      </c>
+      <c r="B23">
+        <v>6.32254767417907</v>
+      </c>
+      <c r="D23" t="s">
+        <v>271</v>
+      </c>
+      <c r="E23">
+        <v>7.4669864177703804</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>272</v>
+      </c>
+      <c r="B24">
+        <v>2.24234914779663</v>
+      </c>
+      <c r="D24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E24">
+        <v>4.2333745956420898</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>273</v>
+      </c>
+      <c r="B25">
+        <v>4.7645616531371999</v>
+      </c>
+      <c r="D25" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25">
+        <v>5.42059326171875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>274</v>
+      </c>
+      <c r="B26">
+        <v>4.4594156742095903</v>
+      </c>
+      <c r="D26" t="s">
+        <v>274</v>
+      </c>
+      <c r="E26">
+        <v>5.0144405364990199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>275</v>
+      </c>
+      <c r="B28">
+        <v>3.8300678730010902</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>276</v>
+      </c>
+      <c r="B29">
+        <v>4.0121998786926198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B30">
+        <v>3.8441522121429399</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>278</v>
+      </c>
+      <c r="B31">
+        <v>4.3123424053192103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B32">
+        <v>4.0654783248901296</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B33">
+        <v>4.2319996356964102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>281</v>
+      </c>
+      <c r="B34">
+        <v>3.46641540527343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>282</v>
+      </c>
+      <c r="B35">
+        <v>2.2143316268920898</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>283</v>
+      </c>
+      <c r="B36">
+        <v>2.6532278060913002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>284</v>
+      </c>
+      <c r="B37">
+        <v>2.2639787197113002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>285</v>
+      </c>
+      <c r="B38">
+        <v>2.4980709552764799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>286</v>
+      </c>
+      <c r="B39">
+        <v>2.2948737144470202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>287</v>
+      </c>
+      <c r="B41">
+        <v>2.90517878532409</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>288</v>
+      </c>
+      <c r="B42">
+        <v>346.88626980781498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>289</v>
+      </c>
+      <c r="B43">
+        <v>609.64147663116398</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>290</v>
+      </c>
+      <c r="B44">
+        <v>4.0512599945068297</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>291</v>
+      </c>
+      <c r="B45">
+        <v>12.465900897979701</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>292</v>
+      </c>
+      <c r="B46">
+        <v>12.5259017944335</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>293</v>
+      </c>
+      <c r="B47">
+        <v>3.6356956958770699</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>294</v>
+      </c>
+      <c r="B48">
+        <v>369.38288593292202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>295</v>
+      </c>
+      <c r="B49">
+        <v>326.88774418830798</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>296</v>
+      </c>
+      <c r="B50">
+        <v>1.74955534934997</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>297</v>
+      </c>
+      <c r="B51">
+        <v>6.09236359596252</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>298</v>
+      </c>
+      <c r="B52">
+        <v>5.8266966342925999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54">
+        <v>4.0302970409393302</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55">
+        <v>3.9522206783294598</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56">
+        <v>3.9521634578704798</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57">
+        <v>4.2177505493164</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58">
+        <v>4.0615775585174498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59">
+        <v>4.1084048748016304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>98</v>
+      </c>
+      <c r="B60">
+        <v>1.7495892047882</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61">
+        <v>1.64023041725158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62">
+        <v>1.6544482707977199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63">
+        <v>1.7808289527893</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64">
+        <v>2.0620136260986301</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>121</v>
+      </c>
+      <c r="B65">
+        <v>1.7626423835754299</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>299</v>
+      </c>
+      <c r="B67">
+        <v>4.2007796764373699</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>300</v>
+      </c>
+      <c r="B68">
+        <v>14.1896810531616</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>301</v>
+      </c>
+      <c r="B69">
+        <v>17.3211476802825</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>302</v>
+      </c>
+      <c r="B70">
+        <v>4.1845605373382497</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>303</v>
+      </c>
+      <c r="B71">
+        <v>5.8505806922912598</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>304</v>
+      </c>
+      <c r="B72">
+        <v>5.9193437099456698</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>305</v>
+      </c>
+      <c r="B73">
+        <v>1.7578601837158201</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>306</v>
+      </c>
+      <c r="B74">
+        <v>11.605495929718</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>307</v>
+      </c>
+      <c r="B75">
+        <v>14.9308655261993</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>308</v>
+      </c>
+      <c r="B76">
+        <v>1.7783782482147199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>309</v>
+      </c>
+      <c r="B77">
+        <v>3.5441079139709402</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>310</v>
+      </c>
+      <c r="B78">
+        <v>3.5071156024932799</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B80">
+        <v>12.5540857315063</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B81">
+        <v>12.7453706264495</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B82">
+        <v>12.760683059692299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B83">
+        <v>12.62047457695</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B84">
+        <v>13.760821104049599</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>13.807446241378701</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86">
+        <v>12.589291572570801</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87">
+        <v>13.042328119277901</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="B88">
+        <v>12.714251279830901</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="B89">
+        <v>12.4807922840118</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="B90">
+        <v>13.496390342712401</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="B91">
+        <v>13.075347185134801</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+      <c r="B93">
+        <v>13.7766642570495</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="B94">
+        <v>17.1676135063171</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3">
-        <v>9800546884536740</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="B95">
+        <v>17.759673357009799</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>326</v>
+      </c>
+      <c r="B96">
+        <v>13.1993441581726</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+      <c r="B97">
+        <v>11.558161973953201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="3">
-        <v>1.27781951427459E+16</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+      <c r="B98">
+        <v>11.495925188064501</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>329</v>
+      </c>
+      <c r="B99">
+        <v>13.3825185298919</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="B100">
+        <v>17.400565147399899</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="B101">
+        <v>17.6986820697784</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+        <v>332</v>
+      </c>
+      <c r="B102">
+        <v>13.026650905609101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="B103">
+        <v>11.654093027114801</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="3">
-        <v>1.95266389846801E+16</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+      <c r="B104">
+        <v>11.412866353988599</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="3">
-        <v>1.89017796516418E+16</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="3">
-        <v>9685242176055900</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="3">
-        <v>1.28719611167907E+16</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="3">
-        <v>1.93704485893249E+16</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="3">
-        <v>1.90580034255981E+16</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>364</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC6ADA2-E968-4884-BF6C-A9714FCD2FE2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>